<commit_message>
Refazendo os gráficos de história de vida e demografia
</commit_message>
<xml_diff>
--- a/Shortfall_data.xlsx
+++ b/Shortfall_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\OneDrive - unb.br\Doutorado\CapI\Dados_analises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\OneDrive - unb.br\Doutorado\CapI\Analises\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7944" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7944"/>
   </bookViews>
   <sheets>
     <sheet name="Demografia" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="313">
   <si>
     <t>ID</t>
   </si>
@@ -963,6 +963,12 @@
   </si>
   <si>
     <t>BodyMass(min)</t>
+  </si>
+  <si>
+    <t>AdultSexratio</t>
+  </si>
+  <si>
+    <t>BirthSexratio</t>
   </si>
 </sst>
 </file>
@@ -1305,9 +1311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1390,13 +1396,13 @@
         <v>241</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>242</v>
+        <v>311</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>243</v>
       </c>
       <c r="R1" t="s">
-        <v>244</v>
+        <v>312</v>
       </c>
       <c r="S1" t="s">
         <v>245</v>
@@ -6401,7 +6407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>